<commit_message>
fixes to arc reactor
</commit_message>
<xml_diff>
--- a/Info/ItemsPerMin.xlsx
+++ b/Info/ItemsPerMin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Refined E65</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Adv Reactor Core</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Reactor Coolant</t>
   </si>
 </sst>
 </file>
@@ -144,11 +150,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -162,6 +165,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,7 +456,7 @@
   <dimension ref="C3:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,401 +470,429 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>(60/I$4)*D4</f>
         <v>80</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
         <v>4000</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="7">
         <f>(60/I$4)*G4</f>
         <v>40000</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>5000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f>(60/I$4)*D5</f>
         <v>50000</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>3000</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f>(60/I$7)*D7</f>
         <v>30000</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="6">
         <v>2000</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="7">
         <f>(60/I$7)*G7</f>
         <v>20000</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>10</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f>(60/I$7)*D8</f>
         <v>100</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>2000</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f>(60/I$10)*D10</f>
         <v>6000</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="6">
         <v>1000</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="7">
         <f>(60/I$10)*G10</f>
         <v>3000</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>30</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f>(60/I$10)*D11</f>
         <v>90</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="1"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>3000</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f>(60/I$13)*D13</f>
         <v>3000</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="6">
         <v>20</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="7">
         <f>(60/I$13)*G13</f>
         <v>20</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="6">
         <v>60</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>20</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f>(60/I$13)*D14</f>
         <v>20</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="2"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="3">
+        <f>(60/I$16)*D16</f>
+        <v>30000</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H16" s="7">
+        <f>(60/I$16)*G16</f>
+        <v>3000</v>
+      </c>
+      <c r="I16" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
@@ -864,14 +901,6 @@
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="I13:I14"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Arc Reactor UI
</commit_message>
<xml_diff>
--- a/Info/ItemsPerMin.xlsx
+++ b/Info/ItemsPerMin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Refined E65</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>Reactor Coolant</t>
+  </si>
+  <si>
+    <t>LimeStone</t>
+  </si>
+  <si>
+    <t>Coolant Powder</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Baux</t>
+  </si>
+  <si>
+    <t>Cloudy Coolant</t>
+  </si>
+  <si>
+    <t>Empty Canister</t>
+  </si>
+  <si>
+    <t>Quartz Crystals</t>
+  </si>
+  <si>
+    <t>Heavy Modular Frame</t>
   </si>
 </sst>
 </file>
@@ -150,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -165,6 +189,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -453,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:I34"/>
+  <dimension ref="C3:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,24 +533,24 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <f>(60/I$4)*D4</f>
-        <v>80</v>
-      </c>
-      <c r="F4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="6">
-        <v>4000</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="G4" s="10">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="11">
         <f>(60/I$4)*G4</f>
-        <v>40000</v>
-      </c>
-      <c r="I4" s="6">
-        <v>6</v>
+        <v>20000</v>
+      </c>
+      <c r="I4" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -522,16 +558,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="2">
         <f>(60/I$4)*D5</f>
-        <v>50000</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="6"/>
+        <v>20000</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
@@ -547,24 +583,24 @@
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="E7" s="2">
         <f>(60/I$7)*D7</f>
-        <v>30000</v>
-      </c>
-      <c r="F7" s="6" t="s">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6">
-        <v>2000</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="G7" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="11">
         <f>(60/I$7)*G7</f>
         <v>20000</v>
       </c>
-      <c r="I7" s="6">
-        <v>6</v>
+      <c r="I7" s="10">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
@@ -576,12 +612,12 @@
       </c>
       <c r="E8" s="2">
         <f>(60/I$7)*D8</f>
-        <v>100</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
@@ -597,24 +633,24 @@
         <v>11</v>
       </c>
       <c r="D10" s="1">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="2">
         <f>(60/I$10)*D10</f>
-        <v>6000</v>
-      </c>
-      <c r="F10" s="6" t="s">
+        <v>20000</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="8">
         <v>1000</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="9">
         <f>(60/I$10)*G10</f>
-        <v>3000</v>
-      </c>
-      <c r="I10" s="6">
-        <v>20</v>
+        <v>20000</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
@@ -622,66 +658,73 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2">
         <f>(60/I$10)*D11</f>
-        <v>90</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="8">
+        <v>2</v>
+      </c>
+      <c r="H11" s="9">
+        <f>(60/I$10)*G11</f>
+        <v>40</v>
+      </c>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3000</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="C13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="8">
+        <v>10</v>
+      </c>
+      <c r="E13" s="9">
         <f>(60/I$13)*D13</f>
-        <v>3000</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="6">
-        <v>20</v>
-      </c>
-      <c r="H13" s="7">
+        <v>100</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11">
         <f>(60/I$13)*G13</f>
-        <v>20</v>
-      </c>
-      <c r="I13" s="6">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="I13" s="10">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1">
-        <v>20</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
         <f>(60/I$13)*D14</f>
-        <v>20</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -694,118 +737,194 @@
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E16" s="2">
+        <f>(60/I$16)*D16</f>
         <v>10000</v>
       </c>
-      <c r="E16" s="3">
-        <f>(60/I$16)*D16</f>
-        <v>30000</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1000</v>
-      </c>
-      <c r="H16" s="7">
+      <c r="F16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11">
         <f>(60/I$16)*G16</f>
-        <v>3000</v>
-      </c>
-      <c r="I16" s="6">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="I16" s="10">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="6"/>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <f>(60/I$16)*D17</f>
+        <v>5</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3">
+        <f>(60/I$19)*D19</f>
+        <v>40</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="10">
+        <v>5</v>
+      </c>
+      <c r="H19" s="11">
+        <f>(60/I$19)*G19</f>
+        <v>100</v>
+      </c>
+      <c r="I19" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <f>(60/I$19)*D20</f>
+        <v>20</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="7">
+        <f>(60/I$19)*D21</f>
+        <v>40</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="7">
+        <f>(60/I$23)*D23</f>
+        <v>5000</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1000</v>
+      </c>
+      <c r="H23" s="11">
+        <f>(60/I$23)*G23</f>
+        <v>5000</v>
+      </c>
+      <c r="I23" s="10">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="C24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="6">
+        <v>20</v>
+      </c>
+      <c r="E24" s="7">
+        <f>(60/I$23)*D24</f>
+        <v>100</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="7"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="C26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="7">
+        <f>(60/I$26)*D26</f>
+        <v>2500</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="7">
+        <f>(60/I$26)*G26</f>
+        <v>2500</v>
+      </c>
+      <c r="I26" s="6">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
@@ -879,12 +998,31 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
+  <mergeCells count="25">
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="I4:I5"/>
@@ -893,14 +1031,18 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>